<commit_message>
added new vocab, fixed endings for numerous regions and tenses.
</commit_message>
<xml_diff>
--- a/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
+++ b/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="367">
   <si>
     <t xml:space="preserve">Laz Infinitive</t>
   </si>
@@ -939,6 +939,117 @@
   </si>
   <si>
     <t xml:space="preserve">çamums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to feed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yedirmek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oʒ̆ilu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆ilums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆iloms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆ilups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to pluck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koparmak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oxu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to shovel up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">küremek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oxop̌u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xop̌ups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ocoxu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ucoxams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ucoxops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to call someone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">çağırmak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oyoxu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uyoxums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to grind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">öğütmek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oğuru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ğurun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to die</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ölmek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oʒ̆odu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆odums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">örmek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oʒ̆k̆idu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆k̆idums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ̆k̆idups</t>
   </si>
   <si>
     <t xml:space="preserve">Category:</t>
@@ -1111,28 +1222,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1432,12 +1551,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE81"/>
+  <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3259,6 +3378,222 @@
       </c>
       <c r="D81" s="3" t="s">
         <v>278</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3294,145 +3629,145 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="32.42"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>307</v>
+      <c r="A2" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>311</v>
+      <c r="B5" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>313</v>
+      <c r="A8" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>314</v>
+      <c r="B9" s="7" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>315</v>
+      <c r="B10" s="7" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>316</v>
+      <c r="B11" s="7" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>317</v>
+      <c r="B12" s="7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>318</v>
+      <c r="B13" s="7" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>319</v>
+      <c r="A14" s="7" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>321</v>
+      <c r="A15" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>323</v>
+      <c r="A16" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>325</v>
+      <c r="A17" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>327</v>
+      <c r="A18" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>329</v>
+      <c r="A19" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more bug fixes for meşvelu
</commit_message>
<xml_diff>
--- a/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
+++ b/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Lazverbcon\laz_verb_conjugator\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1578C7-D84A-4CEF-B230-02E3954B2533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F9D08-9596-42F9-9CF8-F12CE8F2AF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="1510" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1261,12 +1261,6 @@
     <t>meşvelu</t>
   </si>
   <si>
-    <t>şvelams</t>
-  </si>
-  <si>
-    <t>şvelaps</t>
-  </si>
-  <si>
     <t>to help</t>
   </si>
   <si>
@@ -1349,6 +1343,12 @@
   </si>
   <si>
     <t>Çxala-Hopa</t>
+  </si>
+  <si>
+    <t>nuşvelams</t>
+  </si>
+  <si>
+    <t>nuşvelaps</t>
   </si>
 </sst>
 </file>
@@ -4248,22 +4248,22 @@
         <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E109" t="s">
+        <v>439</v>
+      </c>
+      <c r="F109" t="s">
+        <v>23</v>
+      </c>
+      <c r="I109" t="s">
+        <v>410</v>
+      </c>
+      <c r="J109" t="s">
         <v>411</v>
-      </c>
-      <c r="F109" t="s">
-        <v>23</v>
-      </c>
-      <c r="I109" t="s">
-        <v>412</v>
-      </c>
-      <c r="J109" t="s">
-        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -4297,13 +4297,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2" t="s">
         <v>414</v>
-      </c>
-      <c r="B2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4311,10 +4311,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4322,7 +4322,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
@@ -4333,7 +4333,7 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C5" t="s">
         <v>232</v>
@@ -4341,10 +4341,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4352,7 +4352,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4368,7 +4368,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4376,7 +4376,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4384,7 +4384,7 @@
         <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4392,52 +4392,52 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B20" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B21" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B24" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed ivd verbs ending in 'rs', fixed doguru conjugations.
</commit_message>
<xml_diff>
--- a/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
+++ b/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Lazverbcon\laz_verb_conjugator\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F9D08-9596-42F9-9CF8-F12CE8F2AF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2910D6D-A5AB-448A-A85A-1B5FF6C56C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="1510" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -862,9 +862,6 @@
     <t>iqven</t>
   </si>
   <si>
-    <t>oropumu</t>
-  </si>
-  <si>
     <t>aoropen</t>
   </si>
   <si>
@@ -1349,6 +1346,9 @@
   </si>
   <si>
     <t>nuşvelaps</t>
+  </si>
+  <si>
+    <t>oropu</t>
   </si>
 </sst>
 </file>
@@ -1686,9 +1686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" zoomScale="320" zoomScaleNormal="320" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3296,13 +3296,13 @@
     </row>
     <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>277</v>
+        <v>439</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>18</v>
@@ -3316,19 +3316,19 @@
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -3342,91 +3342,91 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E69" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F69" t="s">
         <v>28</v>
       </c>
       <c r="G69" t="s">
+        <v>284</v>
+      </c>
+      <c r="H69" t="s">
+        <v>23</v>
+      </c>
+      <c r="I69" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="H69" t="s">
-        <v>23</v>
-      </c>
-      <c r="I69" s="3" t="s">
+      <c r="J69" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E70" t="s">
+        <v>289</v>
+      </c>
+      <c r="F70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" t="s">
         <v>290</v>
-      </c>
-      <c r="F70" t="s">
-        <v>23</v>
-      </c>
-      <c r="G70" t="s">
-        <v>291</v>
       </c>
       <c r="H70" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I71" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>11</v>
@@ -3450,13 +3450,13 @@
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>298</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" t="s">
         <v>299</v>
-      </c>
-      <c r="B73" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" t="s">
-        <v>300</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
@@ -3464,13 +3464,13 @@
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>302</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>59</v>
@@ -3480,27 +3480,27 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="J74" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>304</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" t="s">
         <v>305</v>
       </c>
-      <c r="B75" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>306</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>307</v>
-      </c>
-      <c r="E75" t="s">
-        <v>308</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -3508,19 +3508,19 @@
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>23</v>
@@ -3528,21 +3528,21 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="J76" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>13</v>
@@ -3552,7 +3552,7 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>134</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -3568,129 +3568,129 @@
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E79" t="s">
+        <v>319</v>
+      </c>
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="I79" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F79" t="s">
-        <v>23</v>
-      </c>
-      <c r="I79" s="3" t="s">
+      <c r="J79" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="J79" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>324</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F80" s="3"/>
       <c r="J80" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G81" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I81" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="H81" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I81" s="3" t="s">
+      <c r="J81" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I82" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J82" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>102</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>28</v>
@@ -3704,33 +3704,33 @@
     </row>
     <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I85" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="J85" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>342</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>343</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>228</v>
@@ -3748,19 +3748,19 @@
     </row>
     <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>345</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>28</v>
@@ -3768,61 +3768,61 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J87" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>348</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" t="s">
         <v>349</v>
       </c>
-      <c r="B88" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>23</v>
+      </c>
+      <c r="I88" t="s">
         <v>350</v>
       </c>
-      <c r="D88" t="s">
-        <v>23</v>
-      </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>351</v>
-      </c>
-      <c r="J88" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E89" t="s">
+        <v>354</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+      <c r="I89" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="F89" t="s">
-        <v>23</v>
-      </c>
-      <c r="I89" s="3" t="s">
+      <c r="J89" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>52</v>
@@ -3842,33 +3842,33 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>358</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" t="s">
         <v>359</v>
-      </c>
-      <c r="B91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C91" t="s">
-        <v>360</v>
       </c>
       <c r="D91" t="s">
         <v>41</v>
       </c>
       <c r="I91" t="s">
+        <v>350</v>
+      </c>
+      <c r="J91" t="s">
         <v>351</v>
-      </c>
-      <c r="J91" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>23</v>
@@ -3878,67 +3878,67 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J92" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="J92" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E93" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F93" t="s">
         <v>18</v>
       </c>
       <c r="I93" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="J93" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>233</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>367</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" t="s">
         <v>368</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
-      </c>
-      <c r="C95" t="s">
-        <v>369</v>
       </c>
       <c r="D95" t="s">
         <v>13</v>
@@ -3952,283 +3952,283 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>369</v>
+      </c>
+      <c r="B96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" t="s">
         <v>370</v>
-      </c>
-      <c r="B96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C96" t="s">
-        <v>371</v>
       </c>
       <c r="D96" t="s">
         <v>13</v>
       </c>
       <c r="E96" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F96" t="s">
         <v>28</v>
       </c>
       <c r="G96" t="s">
+        <v>372</v>
+      </c>
+      <c r="H96" t="s">
+        <v>23</v>
+      </c>
+      <c r="I96" t="s">
         <v>373</v>
       </c>
-      <c r="H96" t="s">
-        <v>23</v>
-      </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>374</v>
-      </c>
-      <c r="J96" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>375</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" t="s">
         <v>376</v>
-      </c>
-      <c r="B97" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" t="s">
-        <v>377</v>
       </c>
       <c r="D97" t="s">
         <v>28</v>
       </c>
       <c r="E97" t="s">
+        <v>377</v>
+      </c>
+      <c r="F97" t="s">
+        <v>23</v>
+      </c>
+      <c r="I97" t="s">
         <v>378</v>
       </c>
-      <c r="F97" t="s">
-        <v>23</v>
-      </c>
-      <c r="I97" t="s">
+      <c r="J97" t="s">
         <v>379</v>
-      </c>
-      <c r="J97" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
       </c>
       <c r="C98" t="s">
+        <v>381</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
+      <c r="I98" t="s">
         <v>382</v>
       </c>
-      <c r="D98" t="s">
-        <v>23</v>
-      </c>
-      <c r="I98" t="s">
+      <c r="J98" t="s">
         <v>383</v>
-      </c>
-      <c r="J98" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B99" t="s">
         <v>11</v>
       </c>
       <c r="C99" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D99" t="s">
         <v>23</v>
       </c>
       <c r="I99" t="s">
+        <v>382</v>
+      </c>
+      <c r="J99" t="s">
         <v>383</v>
-      </c>
-      <c r="J99" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>385</v>
+      </c>
+      <c r="B100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" t="s">
         <v>386</v>
-      </c>
-      <c r="B100" t="s">
-        <v>11</v>
-      </c>
-      <c r="C100" t="s">
-        <v>387</v>
       </c>
       <c r="D100" t="s">
         <v>13</v>
       </c>
       <c r="I100" t="s">
+        <v>378</v>
+      </c>
+      <c r="J100" t="s">
         <v>379</v>
-      </c>
-      <c r="J100" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B101" t="s">
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D101" t="s">
         <v>41</v>
       </c>
       <c r="I101" t="s">
+        <v>382</v>
+      </c>
+      <c r="J101" t="s">
         <v>383</v>
-      </c>
-      <c r="J101" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C102" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="E102" t="s">
         <v>391</v>
-      </c>
-      <c r="E102" t="s">
-        <v>392</v>
       </c>
       <c r="F102" t="s">
         <v>233</v>
       </c>
       <c r="I102" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="J102" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>132</v>
       </c>
       <c r="I103" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="J103" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>59</v>
       </c>
       <c r="I104" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="J104" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I105" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="J105" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>403</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E107" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I107" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I107" s="3" t="s">
+      <c r="J107" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="J107" s="3" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>23</v>
@@ -4242,28 +4242,28 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B109" t="s">
         <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E109" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F109" t="s">
         <v>23</v>
       </c>
       <c r="I109" t="s">
+        <v>409</v>
+      </c>
+      <c r="J109" t="s">
         <v>410</v>
-      </c>
-      <c r="J109" t="s">
-        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -4297,13 +4297,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
         <v>412</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>413</v>
-      </c>
-      <c r="C2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4311,10 +4311,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C3" t="s">
         <v>415</v>
-      </c>
-      <c r="C3" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4322,7 +4322,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
@@ -4333,7 +4333,7 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C5" t="s">
         <v>232</v>
@@ -4341,10 +4341,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>418</v>
+      </c>
+      <c r="C8" t="s">
         <v>419</v>
-      </c>
-      <c r="C8" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4352,7 +4352,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4368,7 +4368,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4376,7 +4376,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4384,7 +4384,7 @@
         <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4392,52 +4392,52 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>427</v>
+      </c>
+      <c r="B20" t="s">
         <v>428</v>
-      </c>
-      <c r="B20" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>429</v>
+      </c>
+      <c r="B21" t="s">
         <v>430</v>
-      </c>
-      <c r="B21" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>431</v>
+      </c>
+      <c r="B22" t="s">
         <v>432</v>
-      </c>
-      <c r="B22" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>433</v>
+      </c>
+      <c r="B23" t="s">
         <v>434</v>
-      </c>
-      <c r="B23" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>435</v>
+      </c>
+      <c r="B24" t="s">
         <v>436</v>
-      </c>
-      <c r="B24" t="s">
-        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed Ardeşen y issue, tested one drive excel successfully
</commit_message>
<xml_diff>
--- a/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
+++ b/laz_verb_conjugator/notebooks/data/Test Verb Present tense.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Lazverbcon\laz_verb_conjugator\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2910D6D-A5AB-448A-A85A-1B5FF6C56C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{A2910D6D-A5AB-448A-A85A-1B5FF6C56C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E32BBB0-4743-4F5F-941E-39704FE73A72}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$90</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -29,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="445">
   <si>
     <t>Laz Infinitive</t>
   </si>
@@ -862,6 +876,9 @@
     <t>iqven</t>
   </si>
   <si>
+    <t>oropu</t>
+  </si>
+  <si>
     <t>aoropen</t>
   </si>
   <si>
@@ -1258,12 +1275,33 @@
     <t>meşvelu</t>
   </si>
   <si>
+    <t>nuşvelams</t>
+  </si>
+  <si>
+    <t>nuşvelaps</t>
+  </si>
+  <si>
     <t>to help</t>
   </si>
   <si>
     <t>yardım etmek</t>
   </si>
   <si>
+    <t>ok̆itxu</t>
+  </si>
+  <si>
+    <t>ik̆itxams</t>
+  </si>
+  <si>
+    <t>ik̆itxaps</t>
+  </si>
+  <si>
+    <t>to ask/read</t>
+  </si>
+  <si>
+    <t>sormak/okumak</t>
+  </si>
+  <si>
     <t>Category:</t>
   </si>
   <si>
@@ -1340,22 +1378,13 @@
   </si>
   <si>
     <t>Çxala-Hopa</t>
-  </si>
-  <si>
-    <t>nuşvelams</t>
-  </si>
-  <si>
-    <t>nuşvelaps</t>
-  </si>
-  <si>
-    <t>oropu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1684,16 +1713,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE109"/>
+  <dimension ref="A1:AE110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="320" zoomScaleNormal="320" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <pane ySplit="1" topLeftCell="C90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +1775,7 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1766,7 +1795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1786,7 +1815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1806,7 +1835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="15">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1826,7 +1855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="15">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1846,7 +1875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="15">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1870,7 +1899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="15">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1892,7 +1921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="15">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1918,7 +1947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="15">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -1944,7 +1973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="15">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1964,7 +1993,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="15">
       <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
@@ -1984,7 +2013,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="15">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -2004,7 +2033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="15">
       <c r="A14" s="3" t="s">
         <v>64</v>
       </c>
@@ -2024,7 +2053,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="15">
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
@@ -2044,7 +2073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="15">
       <c r="A16" s="3" t="s">
         <v>73</v>
       </c>
@@ -2070,7 +2099,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="15">
       <c r="A17" s="3" t="s">
         <v>78</v>
       </c>
@@ -2096,7 +2125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="15">
       <c r="A18" s="3" t="s">
         <v>81</v>
       </c>
@@ -2122,7 +2151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="15">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -2148,7 +2177,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="15">
       <c r="A20" s="3" t="s">
         <v>89</v>
       </c>
@@ -2168,7 +2197,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="15">
       <c r="A21" s="3" t="s">
         <v>93</v>
       </c>
@@ -2188,7 +2217,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="15">
       <c r="A22" s="3" t="s">
         <v>95</v>
       </c>
@@ -2214,7 +2243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="15">
       <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
@@ -2240,7 +2269,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="15">
       <c r="A24" s="3" t="s">
         <v>106</v>
       </c>
@@ -2260,7 +2289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="15">
       <c r="A25" s="3" t="s">
         <v>107</v>
       </c>
@@ -2280,7 +2309,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -2306,7 +2335,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>115</v>
       </c>
@@ -2332,7 +2361,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>120</v>
       </c>
@@ -2358,7 +2387,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>125</v>
       </c>
@@ -2403,7 +2432,7 @@
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>130</v>
       </c>
@@ -2427,7 +2456,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>135</v>
       </c>
@@ -2453,7 +2482,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>141</v>
       </c>
@@ -2485,7 +2514,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>148</v>
       </c>
@@ -2513,7 +2542,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>153</v>
       </c>
@@ -2533,7 +2562,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>157</v>
       </c>
@@ -2565,7 +2594,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>163</v>
       </c>
@@ -2591,7 +2620,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -2617,7 +2646,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>173</v>
       </c>
@@ -2643,7 +2672,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>178</v>
       </c>
@@ -2669,7 +2698,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>183</v>
       </c>
@@ -2695,7 +2724,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>188</v>
       </c>
@@ -2721,7 +2750,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" t="s">
         <v>193</v>
       </c>
@@ -2741,7 +2770,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>197</v>
       </c>
@@ -2767,7 +2796,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>202</v>
       </c>
@@ -2787,7 +2816,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>206</v>
       </c>
@@ -2815,7 +2844,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>211</v>
       </c>
@@ -2841,7 +2870,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>216</v>
       </c>
@@ -2865,7 +2894,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>219</v>
       </c>
@@ -2889,7 +2918,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31" ht="15.75" customHeight="1">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -2915,7 +2944,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>226</v>
       </c>
@@ -2935,7 +2964,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>231</v>
       </c>
@@ -2955,7 +2984,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>236</v>
       </c>
@@ -2979,7 +3008,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>240</v>
       </c>
@@ -3024,7 +3053,7 @@
       <c r="AD53" s="2"/>
       <c r="AE53" s="2"/>
     </row>
-    <row r="54" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:31" ht="15.75" customHeight="1">
       <c r="A54" t="s">
         <v>243</v>
       </c>
@@ -3044,7 +3073,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:31" ht="15.75" customHeight="1">
       <c r="A55" t="s">
         <v>247</v>
       </c>
@@ -3064,7 +3093,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>249</v>
       </c>
@@ -3080,7 +3109,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>251</v>
       </c>
@@ -3100,7 +3129,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>255</v>
       </c>
@@ -3120,7 +3149,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>257</v>
       </c>
@@ -3144,7 +3173,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>261</v>
       </c>
@@ -3168,7 +3197,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>263</v>
       </c>
@@ -3188,7 +3217,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="15.75" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>265</v>
       </c>
@@ -3212,7 +3241,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>267</v>
       </c>
@@ -3238,7 +3267,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="15.75" customHeight="1">
       <c r="A64" s="3" t="s">
         <v>270</v>
       </c>
@@ -3258,7 +3287,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15.75" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>272</v>
       </c>
@@ -3278,7 +3307,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15.75" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>272</v>
       </c>
@@ -3294,15 +3323,15 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15.75" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>439</v>
+        <v>277</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>18</v>
@@ -3314,21 +3343,21 @@
         <v>230</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15.75" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -3340,93 +3369,93 @@
         <v>177</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15.75" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E69" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F69" t="s">
         <v>28</v>
       </c>
       <c r="G69" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H69" t="s">
         <v>23</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E70" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F70" t="s">
         <v>23</v>
       </c>
       <c r="G70" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H70" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>11</v>
@@ -3448,29 +3477,29 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B73" t="s">
         <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15.75" customHeight="1">
       <c r="A74" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>59</v>
@@ -3480,47 +3509,47 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" customHeight="1">
       <c r="A75" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D75" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E75" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15.75" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>23</v>
@@ -3528,21 +3557,21 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>13</v>
@@ -3552,145 +3581,145 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="15.75" customHeight="1">
       <c r="A78" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15.75" customHeight="1">
       <c r="A79" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E79" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F79" t="s">
         <v>23</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F80" s="3"/>
       <c r="J80" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" customHeight="1">
       <c r="A82" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>102</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15.75" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>28</v>
@@ -3702,35 +3731,35 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15.75" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>228</v>
@@ -3746,21 +3775,21 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15.75" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>28</v>
@@ -3768,61 +3797,61 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15.75" customHeight="1">
       <c r="A88" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B88" t="s">
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D88" t="s">
         <v>23</v>
       </c>
       <c r="I88" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J88" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15.75" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E89" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F89" t="s">
         <v>23</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15.75" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>52</v>
@@ -3840,35 +3869,35 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B91" t="s">
         <v>11</v>
       </c>
       <c r="C91" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D91" t="s">
         <v>41</v>
       </c>
       <c r="I91" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J91" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="15">
       <c r="A92" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>23</v>
@@ -3878,67 +3907,67 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15">
       <c r="A93" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E93" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F93" t="s">
         <v>18</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15">
       <c r="A94" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>233</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B95" t="s">
         <v>11</v>
       </c>
       <c r="C95" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D95" t="s">
         <v>13</v>
@@ -3950,285 +3979,285 @@
         <v>172</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B96" t="s">
         <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D96" t="s">
         <v>13</v>
       </c>
       <c r="E96" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F96" t="s">
         <v>28</v>
       </c>
       <c r="G96" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H96" t="s">
         <v>23</v>
       </c>
       <c r="I96" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J96" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D97" t="s">
         <v>28</v>
       </c>
       <c r="E97" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F97" t="s">
         <v>23</v>
       </c>
       <c r="I97" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="J97" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
       </c>
       <c r="C98" t="s">
+        <v>382</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
+      <c r="I98" t="s">
+        <v>383</v>
+      </c>
+      <c r="J98" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" t="s">
         <v>381</v>
       </c>
-      <c r="D98" t="s">
-        <v>23</v>
-      </c>
-      <c r="I98" t="s">
-        <v>382</v>
-      </c>
-      <c r="J98" t="s">
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>385</v>
+      </c>
+      <c r="D99" t="s">
+        <v>23</v>
+      </c>
+      <c r="I99" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>380</v>
-      </c>
-      <c r="B99" t="s">
-        <v>11</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="J99" t="s">
         <v>384</v>
       </c>
-      <c r="D99" t="s">
-        <v>23</v>
-      </c>
-      <c r="I99" t="s">
-        <v>382</v>
-      </c>
-      <c r="J99" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B100" t="s">
         <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D100" t="s">
         <v>13</v>
       </c>
       <c r="I100" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="J100" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B101" t="s">
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D101" t="s">
         <v>41</v>
       </c>
       <c r="I101" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J101" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="15">
       <c r="A102" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E102" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F102" t="s">
         <v>233</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15">
       <c r="A103" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>132</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="15">
       <c r="A104" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>59</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15">
       <c r="A105" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="15">
       <c r="A106" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="15">
       <c r="A107" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="15">
       <c r="A108" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>23</v>
@@ -4240,30 +4269,56 @@
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B109" t="s">
         <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E109" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="F109" t="s">
         <v>23</v>
       </c>
       <c r="I109" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="J109" t="s">
-        <v>410</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" t="s">
+        <v>414</v>
+      </c>
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" t="s">
+        <v>415</v>
+      </c>
+      <c r="D110" t="s">
+        <v>102</v>
+      </c>
+      <c r="E110" t="s">
+        <v>416</v>
+      </c>
+      <c r="F110" t="s">
+        <v>23</v>
+      </c>
+      <c r="I110" t="s">
+        <v>417</v>
+      </c>
+      <c r="J110" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4288,156 +4343,156 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="B2" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="C2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="C3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="C5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="C8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="B20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B21" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="B22" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="B23" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="B24" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>